<commit_message>
fix issues and upgrade the config table
</commit_message>
<xml_diff>
--- a/config/trading_journal_model.xlsx
+++ b/config/trading_journal_model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Cloud Files\TradingTools\trade_journal_project\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F380199-46F9-4B92-9B9E-839E273E1DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1192F56B-8925-424B-B178-53037AB17747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="64">
   <si>
     <t>Sector</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Worst Trade</t>
   </si>
   <si>
-    <t>Deal Type / Entry Label</t>
-  </si>
-  <si>
     <t>Exit Label</t>
   </si>
   <si>
@@ -220,13 +217,25 @@
   </si>
   <si>
     <t>Max Loss</t>
+  </si>
+  <si>
+    <t>Order Type</t>
+  </si>
+  <si>
+    <t>Transmit Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Entry Label</t>
+  </si>
+  <si>
+    <t>Time in Position</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,22 +281,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FF89100D"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF242444"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -311,13 +304,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0" tint="-4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="0" tint="-4.9989318521683403E-2"/>
@@ -333,7 +319,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -422,12 +408,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF0D0D0D"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -456,8 +436,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9F9F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE79D5F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF79CDB5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBE7D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="39">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -994,6 +1010,45 @@
       </left>
       <right style="thick">
         <color theme="0"/>
+      </right>
+      <top style="medium">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="medium">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="0"/>
+      </top>
+      <bottom style="medium">
+        <color theme="2" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="2" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color theme="2" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thick">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="2" tint="-0.499984740745262"/>
+      </left>
+      <right style="medium">
+        <color theme="2" tint="-0.249977111117893"/>
       </right>
       <top style="medium">
         <color theme="2" tint="-0.249977111117893"/>
@@ -1016,7 +1071,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1029,17 +1084,17 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="7" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="7" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1056,115 +1111,112 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="20" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="22" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="9" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="12" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="8" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="14" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="15" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="15" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="20" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="21" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="22" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="9" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="10" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="12" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="8" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="8" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="14" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="15" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="15" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="28" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="18" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="19" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="18" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="19" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1176,43 +1228,88 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="28" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1227,11 +1324,17 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1242,18 +1345,6 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1263,7 +1354,7 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1275,13 +1366,13 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="19" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="19" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1301,6 +1392,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="35" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="39" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="31" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1319,16 +1419,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
-      <color rgb="FFDD878D"/>
-      <color rgb="FFCD94D0"/>
-      <color rgb="FFF1995D"/>
-      <color rgb="FFFAD2BC"/>
-      <color rgb="FFFFE699"/>
-      <color rgb="FFFFFFCC"/>
-      <color rgb="FFDBB1DD"/>
-      <color rgb="FFF98759"/>
-      <color rgb="FF0D0D0D"/>
-      <color rgb="FF912D05"/>
+      <color rgb="FFFFBE7D"/>
+      <color rgb="FF79CDB5"/>
+      <color rgb="FF4784FF"/>
+      <color rgb="FFA7C4FF"/>
+      <color rgb="FF8BB2FF"/>
+      <color rgb="FF6598FF"/>
+      <color rgb="FFE79D5F"/>
+      <color rgb="FFFFCD2F"/>
+      <color rgb="FFFFD961"/>
+      <color rgb="FFFFCB25"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1605,85 +1705,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AY5"/>
+  <dimension ref="A1:BB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3:J3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="AG12" sqref="AF12:AG12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="51" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="54" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" style="52" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="10.77734375" style="52" customWidth="1"/>
-    <col min="11" max="15" width="12.77734375" style="52" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" style="52" customWidth="1"/>
-    <col min="17" max="22" width="10.77734375" style="52" customWidth="1"/>
-    <col min="23" max="23" width="17.33203125" style="52" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.88671875" style="52" bestFit="1" customWidth="1"/>
-    <col min="25" max="28" width="10.77734375" style="52" customWidth="1"/>
-    <col min="29" max="29" width="24.33203125" style="52" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.44140625" style="52" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="30.6640625" style="52" customWidth="1"/>
-    <col min="32" max="32" width="22.5546875" style="52" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.109375" style="64" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.109375" style="66" bestFit="1" customWidth="1"/>
-    <col min="35" max="41" width="8.88671875" style="5"/>
-    <col min="42" max="51" width="8.88671875" style="6"/>
-    <col min="52" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="50" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="53" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10.7109375" style="51" customWidth="1"/>
+    <col min="11" max="12" width="12.7109375" style="51" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="51" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="12.7109375" style="51" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" style="51" customWidth="1"/>
+    <col min="19" max="24" width="10.7109375" style="51" customWidth="1"/>
+    <col min="25" max="25" width="17.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="10.7109375" style="51" customWidth="1"/>
+    <col min="31" max="31" width="24.28515625" style="51" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.42578125" style="51" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.85546875" style="51" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.7109375" style="51" customWidth="1"/>
+    <col min="35" max="35" width="22.5703125" style="51" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.140625" style="63" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19.140625" style="65" bestFit="1" customWidth="1"/>
+    <col min="38" max="44" width="8.85546875" style="5"/>
+    <col min="45" max="54" width="8.85546875" style="6"/>
+    <col min="55" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:51" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:54" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="71" t="s">
+      <c r="C1" s="79" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
-      <c r="AE1" s="72"/>
-      <c r="AF1" s="72"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="79"/>
+      <c r="AB1" s="79"/>
+      <c r="AC1" s="79"/>
+      <c r="AD1" s="79"/>
+      <c r="AE1" s="79"/>
+      <c r="AF1" s="79"/>
+      <c r="AG1" s="79"/>
+      <c r="AH1" s="79"/>
+      <c r="AI1" s="79"/>
+      <c r="AJ1" s="79"/>
+      <c r="AK1" s="79"/>
       <c r="AL1" s="4"/>
       <c r="AM1" s="4"/>
       <c r="AN1" s="4"/>
       <c r="AO1" s="4"/>
-      <c r="AP1" s="7"/>
-      <c r="AQ1" s="7"/>
-      <c r="AR1" s="7"/>
+      <c r="AP1" s="4"/>
+      <c r="AQ1" s="4"/>
+      <c r="AR1" s="4"/>
       <c r="AS1" s="7"/>
       <c r="AT1" s="7"/>
       <c r="AU1" s="7"/>
@@ -1691,8 +1797,11 @@
       <c r="AW1" s="7"/>
       <c r="AX1" s="7"/>
       <c r="AY1" s="7"/>
-    </row>
-    <row r="2" spans="1:51" s="4" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AZ1" s="7"/>
+      <c r="BA1" s="7"/>
+      <c r="BB1" s="7"/>
+    </row>
+    <row r="2" spans="1:54" s="4" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1722,9 +1831,8 @@
       <c r="AA2" s="3"/>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
-      <c r="AP2" s="7"/>
-      <c r="AQ2" s="7"/>
-      <c r="AR2" s="7"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
       <c r="AS2" s="7"/>
       <c r="AT2" s="7"/>
       <c r="AU2" s="7"/>
@@ -1732,208 +1840,230 @@
       <c r="AW2" s="7"/>
       <c r="AX2" s="7"/>
       <c r="AY2" s="7"/>
-    </row>
-    <row r="3" spans="1:51" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="76" t="s">
+      <c r="AZ2" s="7"/>
+      <c r="BA2" s="7"/>
+      <c r="BB2" s="7"/>
+    </row>
+    <row r="3" spans="1:54" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="90" t="s">
         <v>53</v>
       </c>
-      <c r="D3" s="80" t="s">
+      <c r="D3" s="82" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="78" t="s">
+      <c r="E3" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="78" t="s">
+      <c r="F3" s="92" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="67" t="s">
+      <c r="G3" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67" t="s">
+      <c r="H3" s="89"/>
+      <c r="I3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67" t="s">
+      <c r="J3" s="89"/>
+      <c r="K3" s="75" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67" t="s">
+      <c r="L3" s="76"/>
+      <c r="M3" s="76"/>
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67" t="s">
+      <c r="S3" s="86"/>
+      <c r="T3" s="86"/>
+      <c r="U3" s="86"/>
+      <c r="V3" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67" t="s">
+      <c r="W3" s="78"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="X3" s="67" t="s">
+      <c r="Z3" s="84" t="s">
         <v>13</v>
       </c>
-      <c r="Y3" s="73" t="s">
+      <c r="AA3" s="72" t="s">
         <v>14</v>
       </c>
-      <c r="Z3" s="73"/>
-      <c r="AA3" s="73" t="s">
+      <c r="AB3" s="72"/>
+      <c r="AC3" s="117" t="s">
         <v>17</v>
       </c>
-      <c r="AB3" s="73"/>
-      <c r="AC3" s="73"/>
-      <c r="AD3" s="73"/>
-      <c r="AE3" s="74" t="s">
+      <c r="AD3" s="118"/>
+      <c r="AE3" s="118"/>
+      <c r="AF3" s="118"/>
+      <c r="AG3" s="119"/>
+      <c r="AH3" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI3" s="73" t="s">
+        <v>19</v>
+      </c>
+      <c r="AJ3" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="AF3" s="74" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG3" s="69" t="s">
+      <c r="AK3" s="87" t="s">
+        <v>20</v>
+      </c>
+      <c r="AO3" s="6"/>
+    </row>
+    <row r="4" spans="1:54" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C4" s="91"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="J4" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="AH3" s="69" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL3" s="6"/>
-    </row>
-    <row r="4" spans="1:51" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="77"/>
-      <c r="D4" s="81"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="47" t="s">
+      <c r="L4" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="M4" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="N4" s="68" t="s">
+        <v>6</v>
+      </c>
+      <c r="O4" s="68" t="s">
+        <v>7</v>
+      </c>
+      <c r="P4" s="68" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="68" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" s="69" t="s">
+        <v>23</v>
+      </c>
+      <c r="S4" s="69" t="s">
+        <v>11</v>
+      </c>
+      <c r="T4" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="U4" s="69" t="s">
+        <v>7</v>
+      </c>
+      <c r="V4" s="70" t="s">
+        <v>11</v>
+      </c>
+      <c r="W4" s="70" t="s">
+        <v>12</v>
+      </c>
+      <c r="X4" s="70" t="s">
+        <v>7</v>
+      </c>
+      <c r="Y4" s="85"/>
+      <c r="Z4" s="85"/>
+      <c r="AA4" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="47" t="s">
+      <c r="AB4" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="47" t="s">
-        <v>4</v>
-      </c>
-      <c r="J4" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="K4" s="47" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="N4" s="47" t="s">
-        <v>8</v>
-      </c>
-      <c r="O4" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q4" s="47" t="s">
+      <c r="AC4" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD4" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="R4" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="S4" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="T4" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="U4" s="47" t="s">
-        <v>12</v>
-      </c>
-      <c r="V4" s="47" t="s">
-        <v>7</v>
-      </c>
-      <c r="W4" s="68"/>
-      <c r="X4" s="68"/>
-      <c r="Y4" s="48" t="s">
-        <v>4</v>
-      </c>
-      <c r="Z4" s="48" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA4" s="48" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB4" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC4" s="48" t="s">
+      <c r="AE4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="AD4" s="48" t="s">
+      <c r="AF4" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="AE4" s="75"/>
-      <c r="AF4" s="75"/>
-      <c r="AG4" s="70"/>
-      <c r="AH4" s="70"/>
-    </row>
-    <row r="5" spans="1:51" ht="14.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="49"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="50"/>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
-      <c r="AB5" s="50"/>
-      <c r="AC5" s="50"/>
-      <c r="AD5" s="50"/>
-      <c r="AE5" s="50"/>
-      <c r="AF5" s="50"/>
-      <c r="AG5" s="63"/>
-      <c r="AH5" s="65"/>
+      <c r="AG4" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH4" s="74"/>
+      <c r="AI4" s="74"/>
+      <c r="AJ4" s="81"/>
+      <c r="AK4" s="88"/>
+    </row>
+    <row r="5" spans="1:54" ht="14.45" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="48"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="49"/>
+      <c r="P5" s="49"/>
+      <c r="Q5" s="49"/>
+      <c r="R5" s="49"/>
+      <c r="S5" s="49"/>
+      <c r="T5" s="49"/>
+      <c r="U5" s="49"/>
+      <c r="V5" s="49"/>
+      <c r="W5" s="49"/>
+      <c r="X5" s="49"/>
+      <c r="Y5" s="49"/>
+      <c r="Z5" s="49"/>
+      <c r="AA5" s="49"/>
+      <c r="AB5" s="49"/>
+      <c r="AC5" s="49"/>
+      <c r="AD5" s="49"/>
+      <c r="AE5" s="49"/>
+      <c r="AF5" s="49"/>
+      <c r="AG5" s="49"/>
+      <c r="AH5" s="49"/>
+      <c r="AI5" s="49"/>
+      <c r="AJ5" s="62"/>
+      <c r="AK5" s="64"/>
+    </row>
+    <row r="26" spans="33:34" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AG26" s="53"/>
+      <c r="AH26" s="71"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="C1:AK1"/>
+    <mergeCell ref="AJ3:AJ4"/>
     <mergeCell ref="D3:D4"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="P3:S3"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="C1:AF1"/>
-    <mergeCell ref="X3:X4"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="AA3:AD3"/>
-    <mergeCell ref="K3:O3"/>
-    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="Y3:Y4"/>
+    <mergeCell ref="R3:U3"/>
+    <mergeCell ref="AK3:AK4"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="Z3:Z4"/>
+    <mergeCell ref="AC3:AG3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="AH3:AH4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1948,88 +2078,88 @@
       <selection activeCell="B20" sqref="B20:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="5" width="8.88671875" style="8"/>
-    <col min="6" max="6" width="1.77734375" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="8"/>
-    <col min="8" max="9" width="3.77734375" style="9" customWidth="1"/>
-    <col min="10" max="13" width="8.88671875" style="8"/>
-    <col min="14" max="14" width="0.88671875" style="9" customWidth="1"/>
-    <col min="15" max="22" width="8.88671875" style="8"/>
-    <col min="23" max="23" width="11.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.21875" style="8" customWidth="1"/>
-    <col min="28" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="8.85546875" style="9"/>
+    <col min="2" max="5" width="8.85546875" style="8"/>
+    <col min="6" max="6" width="1.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" style="8"/>
+    <col min="8" max="9" width="3.7109375" style="9" customWidth="1"/>
+    <col min="10" max="13" width="8.85546875" style="8"/>
+    <col min="14" max="14" width="0.85546875" style="9" customWidth="1"/>
+    <col min="15" max="22" width="8.85546875" style="8"/>
+    <col min="23" max="23" width="11.140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.28515625" style="8" customWidth="1"/>
+    <col min="28" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="92" t="s">
+    <row r="2" spans="1:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
+      <c r="C2" s="104"/>
+      <c r="D2" s="104"/>
+      <c r="E2" s="104"/>
+      <c r="F2" s="104"/>
+      <c r="G2" s="104"/>
       <c r="H2" s="23"/>
-      <c r="I2" s="92" t="s">
+      <c r="I2" s="104" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="92"/>
-      <c r="K2" s="92"/>
-      <c r="L2" s="92"/>
-      <c r="M2" s="92"/>
-      <c r="N2" s="92"/>
-      <c r="O2" s="92"/>
-      <c r="P2" s="92"/>
-      <c r="Q2" s="92"/>
-      <c r="R2" s="92"/>
-      <c r="S2" s="92"/>
-      <c r="T2" s="92"/>
-      <c r="U2" s="92"/>
-      <c r="V2" s="92"/>
-      <c r="W2" s="92"/>
-      <c r="X2" s="92"/>
-      <c r="Y2" s="92"/>
-      <c r="Z2" s="92"/>
-      <c r="AA2" s="92"/>
-    </row>
-    <row r="3" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
+      <c r="J2" s="104"/>
+      <c r="K2" s="104"/>
+      <c r="L2" s="104"/>
+      <c r="M2" s="104"/>
+      <c r="N2" s="104"/>
+      <c r="O2" s="104"/>
+      <c r="P2" s="104"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="104"/>
+      <c r="T2" s="104"/>
+      <c r="U2" s="104"/>
+      <c r="V2" s="104"/>
+      <c r="W2" s="104"/>
+      <c r="X2" s="104"/>
+      <c r="Y2" s="104"/>
+      <c r="Z2" s="104"/>
+      <c r="AA2" s="104"/>
+    </row>
+    <row r="3" spans="1:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="104"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
       <c r="H3" s="23"/>
-      <c r="I3" s="92"/>
-      <c r="J3" s="92"/>
-      <c r="K3" s="92"/>
-      <c r="L3" s="92"/>
-      <c r="M3" s="92"/>
-      <c r="N3" s="92"/>
-      <c r="O3" s="92"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="92"/>
-      <c r="T3" s="92"/>
-      <c r="U3" s="92"/>
-      <c r="V3" s="92"/>
-      <c r="W3" s="92"/>
-      <c r="X3" s="92"/>
-      <c r="Y3" s="92"/>
-      <c r="Z3" s="92"/>
-      <c r="AA3" s="92"/>
-    </row>
-    <row r="4" spans="1:27" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
+      <c r="P3" s="104"/>
+      <c r="Q3" s="104"/>
+      <c r="R3" s="104"/>
+      <c r="S3" s="104"/>
+      <c r="T3" s="104"/>
+      <c r="U3" s="104"/>
+      <c r="V3" s="104"/>
+      <c r="W3" s="104"/>
+      <c r="X3" s="104"/>
+      <c r="Y3" s="104"/>
+      <c r="Z3" s="104"/>
+      <c r="AA3" s="104"/>
+    </row>
+    <row r="4" spans="1:27" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -2055,7 +2185,7 @@
       <c r="X4" s="10"/>
       <c r="Y4" s="10"/>
     </row>
-    <row r="5" spans="1:27" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
@@ -2064,54 +2194,54 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="96" t="s">
+      <c r="J5" s="108" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="97"/>
-      <c r="L5" s="98"/>
+      <c r="K5" s="109"/>
+      <c r="L5" s="110"/>
       <c r="M5" s="14"/>
       <c r="N5" s="12"/>
-      <c r="O5" s="55" t="s">
+      <c r="O5" s="54" t="s">
         <v>39</v>
       </c>
-      <c r="P5" s="56" t="s">
+      <c r="P5" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="Q5" s="57" t="s">
+      <c r="Q5" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="R5" s="58" t="s">
+      <c r="R5" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="S5" s="57" t="s">
+      <c r="S5" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="T5" s="58" t="s">
+      <c r="T5" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="U5" s="57" t="s">
+      <c r="U5" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="V5" s="58" t="s">
+      <c r="V5" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="W5" s="57" t="s">
+      <c r="W5" s="56" t="s">
         <v>47</v>
       </c>
-      <c r="X5" s="58" t="s">
+      <c r="X5" s="57" t="s">
         <v>48</v>
       </c>
-      <c r="Y5" s="57" t="s">
+      <c r="Y5" s="56" t="s">
         <v>49</v>
       </c>
-      <c r="Z5" s="58" t="s">
+      <c r="Z5" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="AA5" s="59" t="s">
+      <c r="AA5" s="58" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="4" customFormat="1" ht="4.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" s="4" customFormat="1" ht="4.9000000000000004" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="11"/>
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
@@ -2139,22 +2269,22 @@
       <c r="Z6" s="20"/>
       <c r="AA6" s="20"/>
     </row>
-    <row r="7" spans="1:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="86" t="s">
+    <row r="7" spans="1:27" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="94" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="87"/>
-      <c r="D7" s="87"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="85"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="97"/>
       <c r="G7" s="24"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="93" t="s">
+      <c r="J7" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="95"/>
+      <c r="K7" s="106"/>
+      <c r="L7" s="106"/>
+      <c r="M7" s="107"/>
       <c r="N7" s="15"/>
       <c r="O7" s="27"/>
       <c r="P7" s="28"/>
@@ -2170,22 +2300,22 @@
       <c r="Z7" s="31"/>
       <c r="AA7" s="32"/>
     </row>
-    <row r="8" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="89" t="s">
+    <row r="8" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="90"/>
-      <c r="D8" s="90"/>
-      <c r="E8" s="91"/>
-      <c r="F8" s="85"/>
+      <c r="C8" s="102"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="97"/>
       <c r="G8" s="25"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="62"/>
+      <c r="K8" s="60"/>
+      <c r="L8" s="60"/>
+      <c r="M8" s="61"/>
       <c r="N8" s="16"/>
       <c r="O8" s="33"/>
       <c r="P8" s="34"/>
@@ -2201,22 +2331,22 @@
       <c r="Z8" s="37"/>
       <c r="AA8" s="38"/>
     </row>
-    <row r="9" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="89" t="s">
+    <row r="9" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="101" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="91"/>
-      <c r="F9" s="85"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="97"/>
       <c r="G9" s="25"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="62"/>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="61"/>
       <c r="N9" s="17"/>
       <c r="O9" s="33"/>
       <c r="P9" s="34"/>
@@ -2232,22 +2362,22 @@
       <c r="Z9" s="37"/>
       <c r="AA9" s="38"/>
     </row>
-    <row r="10" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="89" t="s">
+    <row r="10" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="101" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="90"/>
-      <c r="D10" s="90"/>
-      <c r="E10" s="91"/>
-      <c r="F10" s="85"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="103"/>
+      <c r="F10" s="97"/>
       <c r="G10" s="25"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="99" t="s">
+      <c r="J10" s="111" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="100"/>
-      <c r="L10" s="100"/>
-      <c r="M10" s="101"/>
+      <c r="K10" s="112"/>
+      <c r="L10" s="112"/>
+      <c r="M10" s="113"/>
       <c r="N10" s="17"/>
       <c r="O10" s="33"/>
       <c r="P10" s="34"/>
@@ -2263,22 +2393,22 @@
       <c r="Z10" s="37"/>
       <c r="AA10" s="38"/>
     </row>
-    <row r="11" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="82" t="s">
+    <row r="11" spans="1:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="83"/>
-      <c r="D11" s="83"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="85"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="100"/>
+      <c r="F11" s="97"/>
       <c r="G11" s="26"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="102" t="s">
+      <c r="J11" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="K11" s="103"/>
-      <c r="L11" s="103"/>
-      <c r="M11" s="104"/>
+      <c r="K11" s="115"/>
+      <c r="L11" s="115"/>
+      <c r="M11" s="116"/>
       <c r="N11" s="21"/>
       <c r="O11" s="39"/>
       <c r="P11" s="40"/>
@@ -2294,7 +2424,7 @@
       <c r="Z11" s="43"/>
       <c r="AA11" s="44"/>
     </row>
-    <row r="12" spans="1:27" s="4" customFormat="1" ht="7.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" s="4" customFormat="1" ht="7.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11"/>
@@ -2322,24 +2452,24 @@
       <c r="Z12" s="46"/>
       <c r="AA12" s="46"/>
     </row>
-    <row r="13" spans="1:27" s="7" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" s="7" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="87"/>
-      <c r="D13" s="87"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="85"/>
+      <c r="C13" s="95"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="96"/>
+      <c r="F13" s="97"/>
       <c r="G13" s="24"/>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
-      <c r="J13" s="86" t="s">
+      <c r="J13" s="94" t="s">
         <v>32</v>
       </c>
-      <c r="K13" s="87"/>
-      <c r="L13" s="87"/>
-      <c r="M13" s="88"/>
+      <c r="K13" s="95"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="96"/>
       <c r="N13" s="22"/>
       <c r="O13" s="27"/>
       <c r="P13" s="28"/>
@@ -2355,24 +2485,24 @@
       <c r="Z13" s="31"/>
       <c r="AA13" s="32"/>
     </row>
-    <row r="14" spans="1:27" s="7" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" s="7" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
-      <c r="B14" s="89" t="s">
+      <c r="B14" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="91"/>
-      <c r="F14" s="85"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="97"/>
       <c r="G14" s="25"/>
       <c r="H14" s="11"/>
       <c r="I14" s="11"/>
-      <c r="J14" s="89" t="s">
+      <c r="J14" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="K14" s="90"/>
-      <c r="L14" s="90"/>
-      <c r="M14" s="91"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="103"/>
       <c r="N14" s="22"/>
       <c r="O14" s="33"/>
       <c r="P14" s="34"/>
@@ -2388,24 +2518,24 @@
       <c r="Z14" s="37"/>
       <c r="AA14" s="38"/>
     </row>
-    <row r="15" spans="1:27" s="7" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" s="7" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
-      <c r="B15" s="82" t="s">
+      <c r="B15" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="83"/>
-      <c r="D15" s="83"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="85"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="99"/>
+      <c r="E15" s="100"/>
+      <c r="F15" s="97"/>
       <c r="G15" s="26"/>
       <c r="H15" s="11"/>
       <c r="I15" s="11"/>
-      <c r="J15" s="82" t="s">
+      <c r="J15" s="98" t="s">
         <v>34</v>
       </c>
-      <c r="K15" s="83"/>
-      <c r="L15" s="83"/>
-      <c r="M15" s="84"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="100"/>
       <c r="N15" s="22"/>
       <c r="O15" s="39"/>
       <c r="P15" s="40"/>
@@ -2421,7 +2551,7 @@
       <c r="Z15" s="43"/>
       <c r="AA15" s="44"/>
     </row>
-    <row r="16" spans="1:27" s="4" customFormat="1" ht="7.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" s="4" customFormat="1" ht="7.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="11"/>
@@ -2449,23 +2579,23 @@
       <c r="Z16" s="46"/>
       <c r="AA16" s="46"/>
     </row>
-    <row r="17" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="86" t="s">
+    <row r="17" spans="2:27" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="88"/>
-      <c r="F17" s="85"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="96"/>
+      <c r="F17" s="97"/>
       <c r="G17" s="24"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="86" t="s">
+      <c r="J17" s="94" t="s">
         <v>35</v>
       </c>
-      <c r="K17" s="87"/>
-      <c r="L17" s="87"/>
-      <c r="M17" s="88"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="95"/>
+      <c r="M17" s="96"/>
       <c r="N17" s="15"/>
       <c r="O17" s="27"/>
       <c r="P17" s="28"/>
@@ -2481,23 +2611,23 @@
       <c r="Z17" s="31"/>
       <c r="AA17" s="32"/>
     </row>
-    <row r="18" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="82" t="s">
+    <row r="18" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="83"/>
-      <c r="D18" s="83"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="85"/>
+      <c r="C18" s="99"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="100"/>
+      <c r="F18" s="97"/>
       <c r="G18" s="26"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="82" t="s">
+      <c r="J18" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="84"/>
+      <c r="K18" s="99"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="100"/>
       <c r="N18" s="17"/>
       <c r="O18" s="39"/>
       <c r="P18" s="40"/>
@@ -2513,7 +2643,7 @@
       <c r="Z18" s="43"/>
       <c r="AA18" s="44"/>
     </row>
-    <row r="19" spans="2:27" s="4" customFormat="1" ht="7.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:27" s="4" customFormat="1" ht="7.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="11"/>
       <c r="C19" s="11"/>
       <c r="D19" s="11"/>
@@ -2541,23 +2671,23 @@
       <c r="Z19" s="46"/>
       <c r="AA19" s="46"/>
     </row>
-    <row r="20" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="86" t="s">
+    <row r="20" spans="2:27" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="C20" s="87"/>
-      <c r="D20" s="87"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="85"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="96"/>
+      <c r="F20" s="97"/>
       <c r="G20" s="24"/>
       <c r="H20" s="10"/>
       <c r="I20" s="10"/>
-      <c r="J20" s="86" t="s">
+      <c r="J20" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="K20" s="87"/>
-      <c r="L20" s="87"/>
-      <c r="M20" s="88"/>
+      <c r="K20" s="95"/>
+      <c r="L20" s="95"/>
+      <c r="M20" s="96"/>
       <c r="N20" s="15"/>
       <c r="O20" s="27"/>
       <c r="P20" s="28"/>
@@ -2573,23 +2703,23 @@
       <c r="Z20" s="31"/>
       <c r="AA20" s="32"/>
     </row>
-    <row r="21" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="82" t="s">
+    <row r="21" spans="2:27" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="C21" s="83"/>
-      <c r="D21" s="83"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="85"/>
+      <c r="C21" s="99"/>
+      <c r="D21" s="99"/>
+      <c r="E21" s="100"/>
+      <c r="F21" s="97"/>
       <c r="G21" s="26"/>
       <c r="H21" s="10"/>
       <c r="I21" s="10"/>
-      <c r="J21" s="82" t="s">
+      <c r="J21" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="K21" s="83"/>
-      <c r="L21" s="83"/>
-      <c r="M21" s="84"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="99"/>
+      <c r="M21" s="100"/>
       <c r="N21" s="17"/>
       <c r="O21" s="39"/>
       <c r="P21" s="40"/>
@@ -2605,7 +2735,7 @@
       <c r="Z21" s="43"/>
       <c r="AA21" s="44"/>
     </row>
-    <row r="22" spans="2:27" s="4" customFormat="1" ht="7.05" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:27" s="4" customFormat="1" ht="7.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2633,23 +2763,23 @@
       <c r="Z22" s="46"/>
       <c r="AA22" s="46"/>
     </row>
-    <row r="23" spans="2:27" s="9" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="86" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="88"/>
-      <c r="F23" s="85"/>
+    <row r="23" spans="2:27" s="9" customFormat="1" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="94" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="96"/>
+      <c r="F23" s="97"/>
       <c r="G23" s="24"/>
       <c r="H23" s="10"/>
       <c r="I23" s="10"/>
-      <c r="J23" s="86" t="s">
+      <c r="J23" s="94" t="s">
         <v>54</v>
       </c>
-      <c r="K23" s="87"/>
-      <c r="L23" s="87"/>
-      <c r="M23" s="88"/>
+      <c r="K23" s="95"/>
+      <c r="L23" s="95"/>
+      <c r="M23" s="96"/>
       <c r="N23" s="15"/>
       <c r="O23" s="27"/>
       <c r="P23" s="28"/>
@@ -2665,23 +2795,23 @@
       <c r="Z23" s="31"/>
       <c r="AA23" s="32"/>
     </row>
-    <row r="24" spans="2:27" s="9" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="82" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="83"/>
-      <c r="D24" s="83"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="85"/>
+    <row r="24" spans="2:27" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="98" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="100"/>
+      <c r="F24" s="97"/>
       <c r="G24" s="26"/>
       <c r="H24" s="10"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="82" t="s">
+      <c r="J24" s="98" t="s">
         <v>55</v>
       </c>
-      <c r="K24" s="83"/>
-      <c r="L24" s="83"/>
-      <c r="M24" s="84"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="100"/>
       <c r="N24" s="17"/>
       <c r="O24" s="39"/>
       <c r="P24" s="40"/>
@@ -2697,7 +2827,7 @@
       <c r="Z24" s="43"/>
       <c r="AA24" s="44"/>
     </row>
-    <row r="25" spans="2:27" s="9" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:27" s="9" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
@@ -2723,7 +2853,7 @@
       <c r="X25" s="10"/>
       <c r="Y25" s="10"/>
     </row>
-    <row r="26" spans="2:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="10"/>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
@@ -2749,7 +2879,7 @@
       <c r="X26" s="10"/>
       <c r="Y26" s="10"/>
     </row>
-    <row r="27" spans="2:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
@@ -2775,11 +2905,12 @@
       <c r="X27" s="10"/>
       <c r="Y27" s="10"/>
     </row>
-    <row r="28" spans="2:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:27" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="F28" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="J21:M21"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="F23:F24"/>
     <mergeCell ref="J23:M23"/>
@@ -2797,14 +2928,9 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="J10:M10"/>
     <mergeCell ref="J11:M11"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F20:F21"/>
     <mergeCell ref="J20:M20"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="F13:F15"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="B17:E17"/>
     <mergeCell ref="J18:M18"/>
     <mergeCell ref="J13:M13"/>
     <mergeCell ref="J14:M14"/>
@@ -2812,8 +2938,12 @@
     <mergeCell ref="B18:E18"/>
     <mergeCell ref="F17:F18"/>
     <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="F13:F15"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B21:E21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finish initial ibapi sand box
Got order information form trades [only on real time], initial ibapi sand box
</commit_message>
<xml_diff>
--- a/config/trading_journal_model.xlsx
+++ b/config/trading_journal_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Cloud Files\TradingTools\trade_journal_project\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1ThF3tjnlT5brQNNAVMi0xIP8nzVANOj2\Cloud Files\TradingTools\trade_journal_project\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6AEBF6-EBF5-41AE-835C-8223E890B681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801FA80F-9B75-4C91-AA2B-4724C2B43FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trade Log" sheetId="1" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>Transmit Price</t>
   </si>
   <si>
-    <t xml:space="preserve"> Entry Label</t>
-  </si>
-  <si>
     <t>New SP Date and Price</t>
   </si>
   <si>
@@ -232,6 +229,9 @@
   </si>
   <si>
     <t>Days in Position</t>
+  </si>
+  <si>
+    <t>Entry Label</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1074,7 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="120">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1261,6 +1261,60 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="35" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1273,12 +1327,6 @@
     <xf numFmtId="0" fontId="5" fillId="25" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1286,54 +1334,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="35" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="40" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="33" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="34" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="24" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="27" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="25" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1404,6 +1404,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1711,10 +1717,10 @@
   <dimension ref="A1:BC26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="4" topLeftCell="S5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AH10" sqref="AH10"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
@@ -1732,7 +1738,7 @@
     <col min="18" max="18" width="22.5546875" style="51" bestFit="1" customWidth="1"/>
     <col min="19" max="24" width="10.6640625" style="51" customWidth="1"/>
     <col min="25" max="25" width="17.33203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.88671875" style="51" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.88671875" style="121" bestFit="1" customWidth="1"/>
     <col min="27" max="30" width="10.6640625" style="51" customWidth="1"/>
     <col min="31" max="31" width="24.33203125" style="51" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="24.33203125" style="51" customWidth="1"/>
@@ -1750,44 +1756,44 @@
     <row r="1" spans="1:55" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-      <c r="L1" s="82"/>
-      <c r="M1" s="82"/>
-      <c r="N1" s="82"/>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="82"/>
-      <c r="R1" s="82"/>
-      <c r="S1" s="82"/>
-      <c r="T1" s="82"/>
-      <c r="U1" s="82"/>
-      <c r="V1" s="82"/>
-      <c r="W1" s="82"/>
-      <c r="X1" s="82"/>
-      <c r="Y1" s="82"/>
-      <c r="Z1" s="82"/>
-      <c r="AA1" s="82"/>
-      <c r="AB1" s="82"/>
-      <c r="AC1" s="82"/>
-      <c r="AD1" s="82"/>
-      <c r="AE1" s="82"/>
-      <c r="AF1" s="82"/>
-      <c r="AG1" s="82"/>
-      <c r="AH1" s="82"/>
-      <c r="AI1" s="82"/>
-      <c r="AJ1" s="82"/>
-      <c r="AK1" s="82"/>
-      <c r="AL1" s="82"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
+      <c r="X1" s="75"/>
+      <c r="Y1" s="75"/>
+      <c r="Z1" s="75"/>
+      <c r="AA1" s="75"/>
+      <c r="AB1" s="75"/>
+      <c r="AC1" s="75"/>
+      <c r="AD1" s="75"/>
+      <c r="AE1" s="75"/>
+      <c r="AF1" s="75"/>
+      <c r="AG1" s="75"/>
+      <c r="AH1" s="75"/>
+      <c r="AI1" s="75"/>
+      <c r="AJ1" s="75"/>
+      <c r="AK1" s="75"/>
+      <c r="AL1" s="75"/>
       <c r="AM1" s="4"/>
       <c r="AN1" s="4"/>
       <c r="AO1" s="4"/>
@@ -1851,83 +1857,83 @@
       <c r="BC2" s="7"/>
     </row>
     <row r="3" spans="1:55" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="93" t="s">
+      <c r="C3" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="D3" s="78" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="92" t="s">
+      <c r="G3" s="85" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="92"/>
-      <c r="I3" s="92" t="s">
+      <c r="H3" s="85"/>
+      <c r="I3" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="92"/>
-      <c r="K3" s="78" t="s">
+      <c r="J3" s="85"/>
+      <c r="K3" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="79"/>
-      <c r="N3" s="79"/>
-      <c r="O3" s="79"/>
-      <c r="P3" s="79"/>
-      <c r="Q3" s="80"/>
-      <c r="R3" s="89" t="s">
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="96"/>
+      <c r="R3" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="89"/>
-      <c r="T3" s="89"/>
-      <c r="U3" s="89"/>
-      <c r="V3" s="81" t="s">
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="81"/>
-      <c r="X3" s="81"/>
-      <c r="Y3" s="87" t="s">
+      <c r="W3" s="72"/>
+      <c r="X3" s="72"/>
+      <c r="Y3" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="Z3" s="87" t="s">
+      <c r="Z3" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="75" t="s">
+      <c r="AA3" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="75"/>
-      <c r="AC3" s="72" t="s">
+      <c r="AB3" s="93"/>
+      <c r="AC3" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="AD3" s="73"/>
-      <c r="AE3" s="73"/>
-      <c r="AF3" s="73"/>
-      <c r="AG3" s="73"/>
-      <c r="AH3" s="74"/>
-      <c r="AI3" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ3" s="76" t="s">
+      <c r="AD3" s="91"/>
+      <c r="AE3" s="91"/>
+      <c r="AF3" s="91"/>
+      <c r="AG3" s="91"/>
+      <c r="AH3" s="92"/>
+      <c r="AI3" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ3" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="AK3" s="83" t="s">
+      <c r="AK3" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="AL3" s="90" t="s">
+      <c r="AL3" s="83" t="s">
         <v>19</v>
       </c>
       <c r="AP3" s="6"/>
     </row>
     <row r="4" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="94"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="96"/>
-      <c r="F4" s="96"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
       <c r="G4" s="67" t="s">
         <v>4</v>
       </c>
@@ -1962,7 +1968,7 @@
         <v>22</v>
       </c>
       <c r="R4" s="69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S4" s="69" t="s">
         <v>11</v>
@@ -1982,8 +1988,8 @@
       <c r="X4" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="88"/>
+      <c r="Y4" s="81"/>
+      <c r="Z4" s="81"/>
       <c r="AA4" s="66" t="s">
         <v>4</v>
       </c>
@@ -1997,21 +2003,21 @@
         <v>11</v>
       </c>
       <c r="AE4" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF4" s="47" t="s">
         <v>62</v>
-      </c>
-      <c r="AF4" s="47" t="s">
-        <v>63</v>
       </c>
       <c r="AG4" s="47" t="s">
         <v>15</v>
       </c>
       <c r="AH4" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="AI4" s="77"/>
-      <c r="AJ4" s="77"/>
-      <c r="AK4" s="84"/>
-      <c r="AL4" s="91"/>
+        <v>63</v>
+      </c>
+      <c r="AI4" s="74"/>
+      <c r="AJ4" s="74"/>
+      <c r="AK4" s="77"/>
+      <c r="AL4" s="84"/>
     </row>
     <row r="5" spans="1:55" ht="14.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="48"/>
@@ -2037,7 +2043,7 @@
       <c r="W5" s="49"/>
       <c r="X5" s="49"/>
       <c r="Y5" s="49"/>
-      <c r="Z5" s="49"/>
+      <c r="Z5" s="120"/>
       <c r="AA5" s="49"/>
       <c r="AB5" s="49"/>
       <c r="AC5" s="49"/>
@@ -2057,6 +2063,10 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="V3:X3"/>
+    <mergeCell ref="AI3:AI4"/>
     <mergeCell ref="C1:AL1"/>
     <mergeCell ref="AK3:AK4"/>
     <mergeCell ref="D3:D4"/>
@@ -2071,10 +2081,6 @@
     <mergeCell ref="Z3:Z4"/>
     <mergeCell ref="AC3:AH3"/>
     <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="AJ3:AJ4"/>
-    <mergeCell ref="K3:Q3"/>
-    <mergeCell ref="V3:X3"/>
-    <mergeCell ref="AI3:AI4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updating default trading Journal and more
Updating default trading Journal and more
</commit_message>
<xml_diff>
--- a/config/trading_journal_model.xlsx
+++ b/config/trading_journal_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\.shortcut-targets-by-id\1ThF3tjnlT5brQNNAVMi0xIP8nzVANOj2\Cloud Files\TradingTools\trade_journal_project\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801FA80F-9B75-4C91-AA2B-4724C2B43FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69CA4B90-4C3F-403B-90FA-40EBBC53C5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trade Log" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>Sector</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Entry Label</t>
+  </si>
+  <si>
+    <t>Number Sold</t>
   </si>
 </sst>
 </file>
@@ -1074,25 +1077,20 @@
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="8" applyFill="1" applyAlignment="1"/>
@@ -1183,7 +1181,7 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="28" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1261,15 +1259,30 @@
     <xf numFmtId="0" fontId="9" fillId="8" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="28" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1327,14 +1340,14 @@
     <xf numFmtId="0" fontId="5" fillId="25" borderId="25" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="35" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1348,14 +1361,26 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="15" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="19" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1366,27 +1391,6 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="13" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="9" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="17" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="18" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="19" xfId="8" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="12" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1404,12 +1408,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="16" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="8" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -1714,105 +1712,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC26"/>
+  <dimension ref="A1:BD26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="S5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AB8" sqref="AB8"/>
+      <selection pane="bottomRight" activeCell="AG13" sqref="AG13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" thickBottom="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="50" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="53" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="10.6640625" style="51" customWidth="1"/>
-    <col min="11" max="12" width="12.6640625" style="51" customWidth="1"/>
-    <col min="13" max="13" width="15.109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="12.6640625" style="51" customWidth="1"/>
-    <col min="18" max="18" width="22.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="19" max="24" width="10.6640625" style="51" customWidth="1"/>
-    <col min="25" max="25" width="17.33203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.88671875" style="121" bestFit="1" customWidth="1"/>
-    <col min="27" max="30" width="10.6640625" style="51" customWidth="1"/>
-    <col min="31" max="31" width="24.33203125" style="51" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="24.33203125" style="51" customWidth="1"/>
-    <col min="33" max="33" width="13.44140625" style="51" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="22.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="30.6640625" style="51" customWidth="1"/>
-    <col min="36" max="36" width="22.5546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19.109375" style="63" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="19.109375" style="65" bestFit="1" customWidth="1"/>
-    <col min="39" max="45" width="8.88671875" style="5"/>
-    <col min="46" max="55" width="8.88671875" style="6"/>
-    <col min="56" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="16.44140625" style="47" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="50" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10.6640625" style="48" customWidth="1"/>
+    <col min="11" max="12" width="12.6640625" style="48" customWidth="1"/>
+    <col min="13" max="13" width="15.109375" style="48" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="12.6640625" style="48" customWidth="1"/>
+    <col min="18" max="18" width="22.5546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="19" max="24" width="10.6640625" style="48" customWidth="1"/>
+    <col min="25" max="25" width="17.33203125" style="48" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.88671875" style="70" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="10.6640625" style="48" customWidth="1"/>
+    <col min="31" max="31" width="13.33203125" style="48" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.33203125" style="48" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="24.33203125" style="48" customWidth="1"/>
+    <col min="34" max="34" width="13.44140625" style="48" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.5546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="30.6640625" style="48" customWidth="1"/>
+    <col min="37" max="37" width="22.5546875" style="48" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="19.109375" style="60" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="19.109375" style="62" bestFit="1" customWidth="1"/>
+    <col min="40" max="46" width="8.88671875" style="3"/>
+    <col min="47" max="56" width="8.88671875" style="5"/>
+    <col min="57" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:56" s="2" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
-      <c r="C1" s="75" t="s">
+      <c r="C1" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="75"/>
-      <c r="N1" s="75"/>
-      <c r="O1" s="75"/>
-      <c r="P1" s="75"/>
-      <c r="Q1" s="75"/>
-      <c r="R1" s="75"/>
-      <c r="S1" s="75"/>
-      <c r="T1" s="75"/>
-      <c r="U1" s="75"/>
-      <c r="V1" s="75"/>
-      <c r="W1" s="75"/>
-      <c r="X1" s="75"/>
-      <c r="Y1" s="75"/>
-      <c r="Z1" s="75"/>
-      <c r="AA1" s="75"/>
-      <c r="AB1" s="75"/>
-      <c r="AC1" s="75"/>
-      <c r="AD1" s="75"/>
-      <c r="AE1" s="75"/>
-      <c r="AF1" s="75"/>
-      <c r="AG1" s="75"/>
-      <c r="AH1" s="75"/>
-      <c r="AI1" s="75"/>
-      <c r="AJ1" s="75"/>
-      <c r="AK1" s="75"/>
-      <c r="AL1" s="75"/>
-      <c r="AM1" s="4"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
+      <c r="L1" s="77"/>
+      <c r="M1" s="77"/>
+      <c r="N1" s="77"/>
+      <c r="O1" s="77"/>
+      <c r="P1" s="77"/>
+      <c r="Q1" s="77"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="77"/>
+      <c r="T1" s="77"/>
+      <c r="U1" s="77"/>
+      <c r="V1" s="77"/>
+      <c r="W1" s="77"/>
+      <c r="X1" s="77"/>
+      <c r="Y1" s="77"/>
+      <c r="Z1" s="77"/>
+      <c r="AA1" s="77"/>
+      <c r="AB1" s="77"/>
+      <c r="AC1" s="77"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="77"/>
+      <c r="AF1" s="77"/>
+      <c r="AG1" s="77"/>
+      <c r="AH1" s="77"/>
+      <c r="AI1" s="77"/>
+      <c r="AJ1" s="77"/>
+      <c r="AK1" s="77"/>
+      <c r="AL1" s="77"/>
+      <c r="AM1" s="77"/>
       <c r="AN1" s="4"/>
       <c r="AO1" s="4"/>
       <c r="AP1" s="4"/>
       <c r="AQ1" s="4"/>
       <c r="AR1" s="4"/>
       <c r="AS1" s="4"/>
-      <c r="AT1" s="7"/>
-      <c r="AU1" s="7"/>
-      <c r="AV1" s="7"/>
-      <c r="AW1" s="7"/>
-      <c r="AX1" s="7"/>
-      <c r="AY1" s="7"/>
-      <c r="AZ1" s="7"/>
-      <c r="BA1" s="7"/>
-      <c r="BB1" s="7"/>
-      <c r="BC1" s="7"/>
-    </row>
-    <row r="2" spans="1:55" s="4" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AT1" s="4"/>
+      <c r="AU1" s="6"/>
+      <c r="AV1" s="6"/>
+      <c r="AW1" s="6"/>
+      <c r="AX1" s="6"/>
+      <c r="AY1" s="6"/>
+      <c r="AZ1" s="6"/>
+      <c r="BA1" s="6"/>
+      <c r="BB1" s="6"/>
+      <c r="BC1" s="6"/>
+      <c r="BD1" s="6"/>
+    </row>
+    <row r="2" spans="1:56" s="4" customFormat="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1845,242 +1845,248 @@
       <c r="AD2" s="3"/>
       <c r="AE2" s="3"/>
       <c r="AF2" s="3"/>
-      <c r="AT2" s="7"/>
-      <c r="AU2" s="7"/>
-      <c r="AV2" s="7"/>
-      <c r="AW2" s="7"/>
-      <c r="AX2" s="7"/>
-      <c r="AY2" s="7"/>
-      <c r="AZ2" s="7"/>
-      <c r="BA2" s="7"/>
-      <c r="BB2" s="7"/>
-      <c r="BC2" s="7"/>
-    </row>
-    <row r="3" spans="1:55" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C3" s="86" t="s">
+      <c r="AG2" s="3"/>
+      <c r="AU2" s="6"/>
+      <c r="AV2" s="6"/>
+      <c r="AW2" s="6"/>
+      <c r="AX2" s="6"/>
+      <c r="AY2" s="6"/>
+      <c r="AZ2" s="6"/>
+      <c r="BA2" s="6"/>
+      <c r="BB2" s="6"/>
+      <c r="BC2" s="6"/>
+      <c r="BD2" s="6"/>
+    </row>
+    <row r="3" spans="1:56" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C3" s="88" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="80" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="88" t="s">
+      <c r="E3" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="88" t="s">
+      <c r="F3" s="90" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="85" t="s">
+      <c r="G3" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85" t="s">
+      <c r="H3" s="87"/>
+      <c r="I3" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="85"/>
-      <c r="K3" s="94" t="s">
+      <c r="J3" s="87"/>
+      <c r="K3" s="73" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="96"/>
-      <c r="R3" s="82" t="s">
+      <c r="L3" s="74"/>
+      <c r="M3" s="74"/>
+      <c r="N3" s="74"/>
+      <c r="O3" s="74"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="75"/>
+      <c r="R3" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="82"/>
-      <c r="T3" s="82"/>
-      <c r="U3" s="82"/>
-      <c r="V3" s="72" t="s">
+      <c r="S3" s="84"/>
+      <c r="T3" s="84"/>
+      <c r="U3" s="84"/>
+      <c r="V3" s="76" t="s">
         <v>10</v>
       </c>
-      <c r="W3" s="72"/>
-      <c r="X3" s="72"/>
-      <c r="Y3" s="80" t="s">
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="Z3" s="80" t="s">
+      <c r="Z3" s="82" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="93" t="s">
+      <c r="AA3" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="AB3" s="93"/>
-      <c r="AC3" s="90" t="s">
+      <c r="AB3" s="95"/>
+      <c r="AC3" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="AD3" s="91"/>
-      <c r="AE3" s="91"/>
-      <c r="AF3" s="91"/>
-      <c r="AG3" s="91"/>
-      <c r="AH3" s="92"/>
-      <c r="AI3" s="73" t="s">
+      <c r="AD3" s="93"/>
+      <c r="AE3" s="93"/>
+      <c r="AF3" s="93"/>
+      <c r="AG3" s="93"/>
+      <c r="AH3" s="93"/>
+      <c r="AI3" s="94"/>
+      <c r="AJ3" s="71" t="s">
         <v>64</v>
       </c>
-      <c r="AJ3" s="73" t="s">
+      <c r="AK3" s="71" t="s">
         <v>18</v>
       </c>
-      <c r="AK3" s="76" t="s">
+      <c r="AL3" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="AL3" s="83" t="s">
+      <c r="AM3" s="85" t="s">
         <v>19</v>
       </c>
-      <c r="AP3" s="6"/>
-    </row>
-    <row r="4" spans="1:55" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="87"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="67" t="s">
+      <c r="AQ3" s="5"/>
+    </row>
+    <row r="4" spans="1:56" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C4" s="89"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="67" t="s">
+      <c r="H4" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="67" t="s">
+      <c r="I4" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="67" t="s">
+      <c r="J4" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="68" t="s">
+      <c r="K4" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="68" t="s">
+      <c r="L4" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="M4" s="68" t="s">
+      <c r="M4" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="N4" s="68" t="s">
+      <c r="N4" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="68" t="s">
+      <c r="O4" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="68" t="s">
+      <c r="P4" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="68" t="s">
+      <c r="Q4" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="69" t="s">
+      <c r="R4" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="S4" s="69" t="s">
+      <c r="S4" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="T4" s="69" t="s">
+      <c r="T4" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="69" t="s">
+      <c r="U4" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="V4" s="70" t="s">
+      <c r="V4" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="W4" s="70" t="s">
+      <c r="W4" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="X4" s="70" t="s">
+      <c r="X4" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="81"/>
-      <c r="Z4" s="81"/>
-      <c r="AA4" s="66" t="s">
+      <c r="Y4" s="83"/>
+      <c r="Z4" s="83"/>
+      <c r="AA4" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="AB4" s="66" t="s">
+      <c r="AB4" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="AC4" s="47" t="s">
+      <c r="AC4" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="AD4" s="47" t="s">
+      <c r="AD4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="AE4" s="47" t="s">
+      <c r="AE4" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF4" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="AF4" s="47" t="s">
+      <c r="AG4" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="AG4" s="47" t="s">
+      <c r="AH4" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="AH4" s="47" t="s">
+      <c r="AI4" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="AI4" s="74"/>
-      <c r="AJ4" s="74"/>
-      <c r="AK4" s="77"/>
-      <c r="AL4" s="84"/>
-    </row>
-    <row r="5" spans="1:55" ht="14.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C5" s="48"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
-      <c r="M5" s="49"/>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
-      <c r="P5" s="49"/>
-      <c r="Q5" s="49"/>
-      <c r="R5" s="49"/>
-      <c r="S5" s="49"/>
-      <c r="T5" s="49"/>
-      <c r="U5" s="49"/>
-      <c r="V5" s="49"/>
-      <c r="W5" s="49"/>
-      <c r="X5" s="49"/>
-      <c r="Y5" s="49"/>
-      <c r="Z5" s="120"/>
-      <c r="AA5" s="49"/>
-      <c r="AB5" s="49"/>
-      <c r="AC5" s="49"/>
-      <c r="AD5" s="49"/>
-      <c r="AE5" s="49"/>
-      <c r="AF5" s="49"/>
-      <c r="AG5" s="49"/>
-      <c r="AH5" s="49"/>
-      <c r="AI5" s="49"/>
-      <c r="AJ5" s="49"/>
-      <c r="AK5" s="62"/>
-      <c r="AL5" s="64"/>
-    </row>
-    <row r="26" spans="34:35" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="AH26" s="53"/>
-      <c r="AI26" s="71"/>
+      <c r="AJ4" s="72"/>
+      <c r="AK4" s="72"/>
+      <c r="AL4" s="79"/>
+      <c r="AM4" s="86"/>
+    </row>
+    <row r="5" spans="1:56" ht="14.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="45"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="46"/>
+      <c r="L5" s="46"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="46"/>
+      <c r="O5" s="46"/>
+      <c r="P5" s="46"/>
+      <c r="Q5" s="46"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="46"/>
+      <c r="T5" s="46"/>
+      <c r="U5" s="46"/>
+      <c r="V5" s="46"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="46"/>
+      <c r="Y5" s="46"/>
+      <c r="Z5" s="69"/>
+      <c r="AA5" s="46"/>
+      <c r="AB5" s="46"/>
+      <c r="AC5" s="46"/>
+      <c r="AD5" s="46"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="46"/>
+      <c r="AG5" s="46"/>
+      <c r="AH5" s="46"/>
+      <c r="AI5" s="46"/>
+      <c r="AJ5" s="46"/>
+      <c r="AK5" s="46"/>
+      <c r="AL5" s="59"/>
+      <c r="AM5" s="61"/>
+    </row>
+    <row r="26" spans="35:36" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AI26" s="50"/>
+      <c r="AJ26" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="AC3:AI3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AK3:AK4"/>
     <mergeCell ref="K3:Q3"/>
     <mergeCell ref="V3:X3"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="C1:AL1"/>
-    <mergeCell ref="AK3:AK4"/>
+    <mergeCell ref="AJ3:AJ4"/>
+    <mergeCell ref="C1:AM1"/>
+    <mergeCell ref="AL3:AL4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="Y3:Y4"/>
     <mergeCell ref="R3:U3"/>
-    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="AM3:AM4"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="Z3:Z4"/>
-    <mergeCell ref="AC3:AH3"/>
-    <mergeCell ref="AA3:AB3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2097,854 +2103,829 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="5" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="8.88671875" style="4"/>
+    <col min="2" max="5" width="8.88671875" style="6"/>
     <col min="6" max="6" width="1.6640625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="8"/>
-    <col min="8" max="9" width="3.6640625" style="9" customWidth="1"/>
-    <col min="10" max="13" width="8.88671875" style="8"/>
-    <col min="14" max="14" width="0.88671875" style="9" customWidth="1"/>
-    <col min="15" max="22" width="8.88671875" style="8"/>
-    <col min="23" max="23" width="11.109375" style="8" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="8.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.44140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.33203125" style="8" customWidth="1"/>
-    <col min="28" max="16384" width="8.88671875" style="8"/>
+    <col min="7" max="7" width="8.88671875" style="6"/>
+    <col min="8" max="9" width="3.6640625" style="4" customWidth="1"/>
+    <col min="10" max="13" width="8.88671875" style="6"/>
+    <col min="14" max="14" width="0.88671875" style="4" customWidth="1"/>
+    <col min="15" max="22" width="8.88671875" style="6"/>
+    <col min="23" max="23" width="11.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="8.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.33203125" style="6" customWidth="1"/>
+    <col min="28" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F1" s="4"/>
-    </row>
-    <row r="2" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="107" t="s">
+    <row r="1" spans="2:27" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="107" t="s">
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="107"/>
-      <c r="M2" s="107"/>
-      <c r="N2" s="107"/>
-      <c r="O2" s="107"/>
-      <c r="P2" s="107"/>
-      <c r="Q2" s="107"/>
-      <c r="R2" s="107"/>
-      <c r="S2" s="107"/>
-      <c r="T2" s="107"/>
-      <c r="U2" s="107"/>
-      <c r="V2" s="107"/>
-      <c r="W2" s="107"/>
-      <c r="X2" s="107"/>
-      <c r="Y2" s="107"/>
-      <c r="Z2" s="107"/>
-      <c r="AA2" s="107"/>
-    </row>
-    <row r="3" spans="1:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="107"/>
-      <c r="C3" s="107"/>
-      <c r="D3" s="107"/>
-      <c r="E3" s="107"/>
-      <c r="F3" s="107"/>
-      <c r="G3" s="107"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="107"/>
-      <c r="J3" s="107"/>
-      <c r="K3" s="107"/>
-      <c r="L3" s="107"/>
-      <c r="M3" s="107"/>
-      <c r="N3" s="107"/>
-      <c r="O3" s="107"/>
-      <c r="P3" s="107"/>
-      <c r="Q3" s="107"/>
-      <c r="R3" s="107"/>
-      <c r="S3" s="107"/>
-      <c r="T3" s="107"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="107"/>
-      <c r="W3" s="107"/>
-      <c r="X3" s="107"/>
-      <c r="Y3" s="107"/>
-      <c r="Z3" s="107"/>
-      <c r="AA3" s="107"/>
-    </row>
-    <row r="4" spans="1:27" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="10"/>
-      <c r="X4" s="10"/>
-      <c r="Y4" s="10"/>
-    </row>
-    <row r="5" spans="1:27" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="111" t="s">
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
+      <c r="P2" s="103"/>
+      <c r="Q2" s="103"/>
+      <c r="R2" s="103"/>
+      <c r="S2" s="103"/>
+      <c r="T2" s="103"/>
+      <c r="U2" s="103"/>
+      <c r="V2" s="103"/>
+      <c r="W2" s="103"/>
+      <c r="X2" s="103"/>
+      <c r="Y2" s="103"/>
+      <c r="Z2" s="103"/>
+      <c r="AA2" s="103"/>
+    </row>
+    <row r="3" spans="2:27" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="103"/>
+      <c r="C3" s="103"/>
+      <c r="D3" s="103"/>
+      <c r="E3" s="103"/>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="103"/>
+      <c r="J3" s="103"/>
+      <c r="K3" s="103"/>
+      <c r="L3" s="103"/>
+      <c r="M3" s="103"/>
+      <c r="N3" s="103"/>
+      <c r="O3" s="103"/>
+      <c r="P3" s="103"/>
+      <c r="Q3" s="103"/>
+      <c r="R3" s="103"/>
+      <c r="S3" s="103"/>
+      <c r="T3" s="103"/>
+      <c r="U3" s="103"/>
+      <c r="V3" s="103"/>
+      <c r="W3" s="103"/>
+      <c r="X3" s="103"/>
+      <c r="Y3" s="103"/>
+      <c r="Z3" s="103"/>
+      <c r="AA3" s="103"/>
+    </row>
+    <row r="4" spans="2:27" s="4" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+    </row>
+    <row r="5" spans="2:27" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="112"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="54" t="s">
+      <c r="K5" s="108"/>
+      <c r="L5" s="109"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="P5" s="55" t="s">
+      <c r="P5" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="Q5" s="56" t="s">
+      <c r="Q5" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="R5" s="57" t="s">
+      <c r="R5" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="S5" s="56" t="s">
+      <c r="S5" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="T5" s="57" t="s">
+      <c r="T5" s="54" t="s">
         <v>43</v>
       </c>
-      <c r="U5" s="56" t="s">
+      <c r="U5" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="V5" s="57" t="s">
+      <c r="V5" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="W5" s="56" t="s">
+      <c r="W5" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="X5" s="57" t="s">
+      <c r="X5" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="Y5" s="56" t="s">
+      <c r="Y5" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="Z5" s="57" t="s">
+      <c r="Z5" s="54" t="s">
         <v>48</v>
       </c>
-      <c r="AA5" s="58" t="s">
+      <c r="AA5" s="55" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="4" customFormat="1" ht="4.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="20"/>
-      <c r="W6" s="20"/>
-      <c r="X6" s="20"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="20"/>
-      <c r="AA6" s="20"/>
-    </row>
-    <row r="7" spans="1:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="97" t="s">
+    <row r="6" spans="2:27" s="4" customFormat="1" ht="4.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="17"/>
+      <c r="S6" s="17"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+    </row>
+    <row r="7" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="99" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="98"/>
-      <c r="D7" s="98"/>
-      <c r="E7" s="99"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="24"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="108" t="s">
+      <c r="C7" s="100"/>
+      <c r="D7" s="100"/>
+      <c r="E7" s="101"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="21"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="104" t="s">
         <v>25</v>
       </c>
-      <c r="K7" s="109"/>
-      <c r="L7" s="109"/>
-      <c r="M7" s="110"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="28"/>
-      <c r="Q7" s="29"/>
-      <c r="R7" s="28"/>
-      <c r="S7" s="30"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="28"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="28"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="31"/>
-      <c r="AA7" s="32"/>
-    </row>
-    <row r="8" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="104" t="s">
+      <c r="K7" s="105"/>
+      <c r="L7" s="105"/>
+      <c r="M7" s="106"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="27"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="27"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="27"/>
+      <c r="Z7" s="28"/>
+      <c r="AA7" s="29"/>
+    </row>
+    <row r="8" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="110" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="25"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="59" t="s">
+      <c r="C8" s="111"/>
+      <c r="D8" s="111"/>
+      <c r="E8" s="112"/>
+      <c r="F8" s="102"/>
+      <c r="G8" s="22"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="34"/>
-      <c r="Q8" s="35"/>
-      <c r="R8" s="34"/>
-      <c r="S8" s="36"/>
-      <c r="T8" s="34"/>
-      <c r="U8" s="36"/>
-      <c r="V8" s="34"/>
-      <c r="W8" s="36"/>
-      <c r="X8" s="34"/>
-      <c r="Y8" s="36"/>
-      <c r="Z8" s="37"/>
-      <c r="AA8" s="38"/>
-    </row>
-    <row r="9" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="104" t="s">
+      <c r="K8" s="57"/>
+      <c r="L8" s="57"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="30"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="32"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="33"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="33"/>
+      <c r="V8" s="31"/>
+      <c r="W8" s="33"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="33"/>
+      <c r="Z8" s="34"/>
+      <c r="AA8" s="35"/>
+    </row>
+    <row r="9" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="105"/>
-      <c r="D9" s="105"/>
-      <c r="E9" s="106"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="25"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="59" t="s">
+      <c r="C9" s="111"/>
+      <c r="D9" s="111"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="22"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="61"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="36"/>
-      <c r="V9" s="34"/>
-      <c r="W9" s="36"/>
-      <c r="X9" s="34"/>
-      <c r="Y9" s="36"/>
-      <c r="Z9" s="37"/>
-      <c r="AA9" s="38"/>
-    </row>
-    <row r="10" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="104" t="s">
+      <c r="K9" s="57"/>
+      <c r="L9" s="57"/>
+      <c r="M9" s="58"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="30"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="32"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="33"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="33"/>
+      <c r="V9" s="31"/>
+      <c r="W9" s="33"/>
+      <c r="X9" s="31"/>
+      <c r="Y9" s="33"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="35"/>
+    </row>
+    <row r="10" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="106"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="25"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="114" t="s">
+      <c r="C10" s="111"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="112"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="22"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="113" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="115"/>
-      <c r="L10" s="115"/>
-      <c r="M10" s="116"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="35"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="36"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="36"/>
-      <c r="V10" s="34"/>
-      <c r="W10" s="36"/>
-      <c r="X10" s="34"/>
-      <c r="Y10" s="36"/>
-      <c r="Z10" s="37"/>
-      <c r="AA10" s="38"/>
-    </row>
-    <row r="11" spans="1:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="101" t="s">
+      <c r="K10" s="114"/>
+      <c r="L10" s="114"/>
+      <c r="M10" s="115"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="30"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="32"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="33"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="33"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="33"/>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="33"/>
+      <c r="Z10" s="34"/>
+      <c r="AA10" s="35"/>
+    </row>
+    <row r="11" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="103"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="26"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="117" t="s">
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="23"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="116" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="118"/>
-      <c r="L11" s="118"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="21"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="40"/>
-      <c r="Q11" s="41"/>
-      <c r="R11" s="40"/>
-      <c r="S11" s="42"/>
-      <c r="T11" s="40"/>
-      <c r="U11" s="42"/>
-      <c r="V11" s="40"/>
-      <c r="W11" s="42"/>
-      <c r="X11" s="40"/>
-      <c r="Y11" s="42"/>
-      <c r="Z11" s="43"/>
-      <c r="AA11" s="44"/>
-    </row>
-    <row r="12" spans="1:27" s="4" customFormat="1" ht="7.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="45"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="45"/>
-      <c r="S12" s="45"/>
-      <c r="T12" s="45"/>
-      <c r="U12" s="45"/>
-      <c r="V12" s="45"/>
-      <c r="W12" s="45"/>
-      <c r="X12" s="45"/>
-      <c r="Y12" s="45"/>
-      <c r="Z12" s="46"/>
-      <c r="AA12" s="46"/>
-    </row>
-    <row r="13" spans="1:27" s="7" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="97" t="s">
+      <c r="K11" s="117"/>
+      <c r="L11" s="117"/>
+      <c r="M11" s="118"/>
+      <c r="N11" s="18"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="38"/>
+      <c r="R11" s="37"/>
+      <c r="S11" s="39"/>
+      <c r="T11" s="37"/>
+      <c r="U11" s="39"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="39"/>
+      <c r="X11" s="37"/>
+      <c r="Y11" s="39"/>
+      <c r="Z11" s="40"/>
+      <c r="AA11" s="41"/>
+    </row>
+    <row r="12" spans="2:27" s="4" customFormat="1" ht="7.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="42"/>
+      <c r="P12" s="42"/>
+      <c r="Q12" s="42"/>
+      <c r="R12" s="42"/>
+      <c r="S12" s="42"/>
+      <c r="T12" s="42"/>
+      <c r="U12" s="42"/>
+      <c r="V12" s="42"/>
+      <c r="W12" s="42"/>
+      <c r="X12" s="42"/>
+      <c r="Y12" s="42"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+    </row>
+    <row r="13" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="98"/>
-      <c r="D13" s="98"/>
-      <c r="E13" s="99"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="97" t="s">
+      <c r="C13" s="100"/>
+      <c r="D13" s="100"/>
+      <c r="E13" s="101"/>
+      <c r="F13" s="102"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="99" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="98"/>
-      <c r="L13" s="98"/>
-      <c r="M13" s="99"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="30"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="30"/>
-      <c r="V13" s="28"/>
-      <c r="W13" s="30"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="30"/>
-      <c r="Z13" s="31"/>
-      <c r="AA13" s="32"/>
-    </row>
-    <row r="14" spans="1:27" s="7" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="104" t="s">
+      <c r="K13" s="100"/>
+      <c r="L13" s="100"/>
+      <c r="M13" s="101"/>
+      <c r="N13" s="19"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="25"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="25"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="27"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="27"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="27"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="29"/>
+    </row>
+    <row r="14" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="105"/>
-      <c r="D14" s="105"/>
-      <c r="E14" s="106"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="104" t="s">
+      <c r="C14" s="111"/>
+      <c r="D14" s="111"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="110" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
-      <c r="M14" s="106"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="33"/>
-      <c r="P14" s="34"/>
-      <c r="Q14" s="36"/>
-      <c r="R14" s="34"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="34"/>
-      <c r="U14" s="36"/>
-      <c r="V14" s="34"/>
-      <c r="W14" s="36"/>
-      <c r="X14" s="34"/>
-      <c r="Y14" s="36"/>
-      <c r="Z14" s="37"/>
-      <c r="AA14" s="38"/>
-    </row>
-    <row r="15" spans="1:27" s="7" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="101" t="s">
+      <c r="K14" s="111"/>
+      <c r="L14" s="111"/>
+      <c r="M14" s="112"/>
+      <c r="N14" s="19"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="33"/>
+      <c r="T14" s="31"/>
+      <c r="U14" s="33"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="33"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="33"/>
+      <c r="Z14" s="34"/>
+      <c r="AA14" s="35"/>
+    </row>
+    <row r="15" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="102"/>
-      <c r="D15" s="102"/>
-      <c r="E15" s="103"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="101" t="s">
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="96" t="s">
         <v>32</v>
       </c>
-      <c r="K15" s="102"/>
-      <c r="L15" s="102"/>
-      <c r="M15" s="103"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="40"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="40"/>
-      <c r="U15" s="42"/>
-      <c r="V15" s="40"/>
-      <c r="W15" s="42"/>
-      <c r="X15" s="40"/>
-      <c r="Y15" s="42"/>
-      <c r="Z15" s="43"/>
-      <c r="AA15" s="44"/>
-    </row>
-    <row r="16" spans="1:27" s="4" customFormat="1" ht="7.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="11"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="45"/>
-      <c r="X16" s="45"/>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="46"/>
-      <c r="AA16" s="46"/>
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="98"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="36"/>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="39"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="39"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="39"/>
+      <c r="Z15" s="40"/>
+      <c r="AA15" s="41"/>
+    </row>
+    <row r="16" spans="2:27" s="4" customFormat="1" ht="7.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="42"/>
+      <c r="V16" s="42"/>
+      <c r="W16" s="42"/>
+      <c r="X16" s="42"/>
+      <c r="Y16" s="42"/>
+      <c r="Z16" s="43"/>
+      <c r="AA16" s="43"/>
     </row>
     <row r="17" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="97" t="s">
+      <c r="B17" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="98"/>
-      <c r="D17" s="98"/>
-      <c r="E17" s="99"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="97" t="s">
+      <c r="C17" s="100"/>
+      <c r="D17" s="100"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="102"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="99" t="s">
         <v>33</v>
       </c>
-      <c r="K17" s="98"/>
-      <c r="L17" s="98"/>
-      <c r="M17" s="99"/>
-      <c r="N17" s="15"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="30"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="30"/>
-      <c r="V17" s="28"/>
-      <c r="W17" s="30"/>
-      <c r="X17" s="28"/>
-      <c r="Y17" s="30"/>
-      <c r="Z17" s="31"/>
-      <c r="AA17" s="32"/>
+      <c r="K17" s="100"/>
+      <c r="L17" s="100"/>
+      <c r="M17" s="101"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="25"/>
+      <c r="Y17" s="27"/>
+      <c r="Z17" s="28"/>
+      <c r="AA17" s="29"/>
     </row>
     <row r="18" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="101" t="s">
+      <c r="B18" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="102"/>
-      <c r="D18" s="102"/>
-      <c r="E18" s="103"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="101" t="s">
+      <c r="C18" s="97"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="K18" s="102"/>
-      <c r="L18" s="102"/>
-      <c r="M18" s="103"/>
-      <c r="N18" s="17"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="40"/>
-      <c r="Q18" s="42"/>
-      <c r="R18" s="40"/>
-      <c r="S18" s="42"/>
-      <c r="T18" s="40"/>
-      <c r="U18" s="42"/>
-      <c r="V18" s="40"/>
-      <c r="W18" s="42"/>
-      <c r="X18" s="40"/>
-      <c r="Y18" s="42"/>
-      <c r="Z18" s="43"/>
-      <c r="AA18" s="44"/>
+      <c r="K18" s="97"/>
+      <c r="L18" s="97"/>
+      <c r="M18" s="98"/>
+      <c r="N18" s="14"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="39"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="39"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="39"/>
+      <c r="V18" s="37"/>
+      <c r="W18" s="39"/>
+      <c r="X18" s="37"/>
+      <c r="Y18" s="39"/>
+      <c r="Z18" s="40"/>
+      <c r="AA18" s="41"/>
     </row>
     <row r="19" spans="2:27" s="4" customFormat="1" ht="7.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-      <c r="U19" s="45"/>
-      <c r="V19" s="45"/>
-      <c r="W19" s="45"/>
-      <c r="X19" s="45"/>
-      <c r="Y19" s="45"/>
-      <c r="Z19" s="46"/>
-      <c r="AA19" s="46"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="42"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="42"/>
+      <c r="R19" s="42"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="42"/>
+      <c r="W19" s="42"/>
+      <c r="X19" s="42"/>
+      <c r="Y19" s="42"/>
+      <c r="Z19" s="43"/>
+      <c r="AA19" s="43"/>
     </row>
     <row r="20" spans="2:27" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="97" t="s">
+      <c r="B20" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="98"/>
-      <c r="D20" s="98"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="97" t="s">
+      <c r="C20" s="100"/>
+      <c r="D20" s="100"/>
+      <c r="E20" s="101"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="K20" s="98"/>
-      <c r="L20" s="98"/>
-      <c r="M20" s="99"/>
-      <c r="N20" s="15"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="28"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="28"/>
-      <c r="S20" s="30"/>
-      <c r="T20" s="28"/>
-      <c r="U20" s="30"/>
-      <c r="V20" s="28"/>
-      <c r="W20" s="30"/>
-      <c r="X20" s="28"/>
-      <c r="Y20" s="30"/>
-      <c r="Z20" s="31"/>
-      <c r="AA20" s="32"/>
+      <c r="K20" s="100"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="101"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="25"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="25"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="25"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="25"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="25"/>
+      <c r="Y20" s="27"/>
+      <c r="Z20" s="28"/>
+      <c r="AA20" s="29"/>
     </row>
     <row r="21" spans="2:27" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="101" t="s">
+      <c r="B21" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="102"/>
-      <c r="D21" s="102"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="101" t="s">
+      <c r="C21" s="97"/>
+      <c r="D21" s="97"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="K21" s="102"/>
-      <c r="L21" s="102"/>
-      <c r="M21" s="103"/>
-      <c r="N21" s="17"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="40"/>
-      <c r="Q21" s="42"/>
-      <c r="R21" s="40"/>
-      <c r="S21" s="42"/>
-      <c r="T21" s="40"/>
-      <c r="U21" s="42"/>
-      <c r="V21" s="40"/>
-      <c r="W21" s="42"/>
-      <c r="X21" s="40"/>
-      <c r="Y21" s="42"/>
-      <c r="Z21" s="43"/>
-      <c r="AA21" s="44"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="14"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="37"/>
+      <c r="S21" s="39"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="39"/>
+      <c r="V21" s="37"/>
+      <c r="W21" s="39"/>
+      <c r="X21" s="37"/>
+      <c r="Y21" s="39"/>
+      <c r="Z21" s="40"/>
+      <c r="AA21" s="41"/>
     </row>
     <row r="22" spans="2:27" s="4" customFormat="1" ht="7.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="45"/>
-      <c r="S22" s="45"/>
-      <c r="T22" s="45"/>
-      <c r="U22" s="45"/>
-      <c r="V22" s="45"/>
-      <c r="W22" s="45"/>
-      <c r="X22" s="45"/>
-      <c r="Y22" s="45"/>
-      <c r="Z22" s="46"/>
-      <c r="AA22" s="46"/>
-    </row>
-    <row r="23" spans="2:27" s="9" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="97" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="42"/>
+      <c r="R22" s="42"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="42"/>
+      <c r="U22" s="42"/>
+      <c r="V22" s="42"/>
+      <c r="W22" s="42"/>
+      <c r="X22" s="42"/>
+      <c r="Y22" s="42"/>
+      <c r="Z22" s="43"/>
+      <c r="AA22" s="43"/>
+    </row>
+    <row r="23" spans="2:27" s="4" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="99" t="s">
         <v>56</v>
       </c>
-      <c r="C23" s="98"/>
-      <c r="D23" s="98"/>
-      <c r="E23" s="99"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="97" t="s">
+      <c r="C23" s="100"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="101"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="99" t="s">
         <v>52</v>
       </c>
-      <c r="K23" s="98"/>
-      <c r="L23" s="98"/>
-      <c r="M23" s="99"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="28"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="28"/>
-      <c r="S23" s="30"/>
-      <c r="T23" s="28"/>
-      <c r="U23" s="30"/>
-      <c r="V23" s="28"/>
-      <c r="W23" s="30"/>
-      <c r="X23" s="28"/>
-      <c r="Y23" s="30"/>
-      <c r="Z23" s="31"/>
-      <c r="AA23" s="32"/>
-    </row>
-    <row r="24" spans="2:27" s="9" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="101" t="s">
+      <c r="K23" s="100"/>
+      <c r="L23" s="100"/>
+      <c r="M23" s="101"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="24"/>
+      <c r="P23" s="25"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="27"/>
+      <c r="T23" s="25"/>
+      <c r="U23" s="27"/>
+      <c r="V23" s="25"/>
+      <c r="W23" s="27"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="28"/>
+      <c r="AA23" s="29"/>
+    </row>
+    <row r="24" spans="2:27" s="4" customFormat="1" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="102"/>
-      <c r="D24" s="102"/>
-      <c r="E24" s="103"/>
-      <c r="F24" s="100"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="101" t="s">
+      <c r="C24" s="97"/>
+      <c r="D24" s="97"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="96" t="s">
         <v>53</v>
       </c>
-      <c r="K24" s="102"/>
-      <c r="L24" s="102"/>
-      <c r="M24" s="103"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="39"/>
-      <c r="P24" s="40"/>
-      <c r="Q24" s="42"/>
-      <c r="R24" s="40"/>
-      <c r="S24" s="42"/>
-      <c r="T24" s="40"/>
-      <c r="U24" s="42"/>
-      <c r="V24" s="40"/>
-      <c r="W24" s="42"/>
-      <c r="X24" s="40"/>
-      <c r="Y24" s="42"/>
-      <c r="Z24" s="43"/>
-      <c r="AA24" s="44"/>
-    </row>
-    <row r="25" spans="2:27" s="9" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
-      <c r="T25" s="10"/>
-      <c r="U25" s="10"/>
-      <c r="V25" s="10"/>
-      <c r="W25" s="10"/>
-      <c r="X25" s="10"/>
-      <c r="Y25" s="10"/>
-    </row>
-    <row r="26" spans="2:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
-      <c r="T26" s="10"/>
-      <c r="U26" s="10"/>
-      <c r="V26" s="10"/>
-      <c r="W26" s="10"/>
-      <c r="X26" s="10"/>
-      <c r="Y26" s="10"/>
-    </row>
-    <row r="27" spans="2:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="10"/>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
-      <c r="T27" s="10"/>
-      <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="10"/>
-    </row>
-    <row r="28" spans="2:27" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="F28" s="4"/>
-    </row>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="98"/>
+      <c r="N24" s="14"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="37"/>
+      <c r="Q24" s="39"/>
+      <c r="R24" s="37"/>
+      <c r="S24" s="39"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="39"/>
+      <c r="V24" s="37"/>
+      <c r="W24" s="39"/>
+      <c r="X24" s="37"/>
+      <c r="Y24" s="39"/>
+      <c r="Z24" s="40"/>
+      <c r="AA24" s="41"/>
+    </row>
+    <row r="25" spans="2:27" s="4" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+    </row>
+    <row r="26" spans="2:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+    </row>
+    <row r="27" spans="2:27" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+    </row>
+    <row r="28" spans="2:27" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="J21:M21"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="I2:AA3"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="B2:G3"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="J11:M11"/>
     <mergeCell ref="B20:E20"/>
     <mergeCell ref="F20:F21"/>
     <mergeCell ref="J20:M20"/>
@@ -2961,6 +2942,24 @@
     <mergeCell ref="J17:M17"/>
     <mergeCell ref="B17:E17"/>
     <mergeCell ref="B21:E21"/>
+    <mergeCell ref="I2:AA3"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="B2:G3"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="J21:M21"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="J24:M24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>